<commit_message>
Thêm sql và chức năng đăng nhập
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TaiLieuHoc\LapTrinh(.)NET\DoAn_DotNet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B829BAB4-BAF9-4902-BF62-DEAE4E196A21}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AD0E592-B3E6-446A-A000-D37E072C5F2B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{D266C75E-4EF3-451E-9F41-2CCBE411A25D}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="38">
   <si>
     <t>CMND</t>
   </si>
@@ -62,9 +62,6 @@
 (ADMIN hoặc NV)</t>
   </si>
   <si>
-    <t>SẢN PHẨM</t>
-  </si>
-  <si>
     <t>LOẠI</t>
   </si>
   <si>
@@ -144,6 +141,15 @@
   </si>
   <si>
     <t>Chi tiết HĐ NHẬP</t>
+  </si>
+  <si>
+    <t>ẢNH</t>
+  </si>
+  <si>
+    <t>HÀNG HÓA</t>
+  </si>
+  <si>
+    <t>MÃ HH</t>
   </si>
 </sst>
 </file>
@@ -206,7 +212,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -229,11 +235,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -268,6 +285,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -584,7 +607,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D22EC28-166D-4546-9605-48C0E8032621}">
-  <dimension ref="A1:J34"/>
+  <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
       <selection activeCell="G21" sqref="G21"/>
@@ -618,9 +641,9 @@
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
     </row>
-    <row r="2" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>4</v>
@@ -632,7 +655,7 @@
         <v>1</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>2</v>
@@ -643,285 +666,304 @@
       <c r="H2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="J2" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5" t="s">
+    <row r="3" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="7"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="14"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="5"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+    </row>
+    <row r="6" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="5"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
+    </row>
+    <row r="13" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="5"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+    </row>
+    <row r="17" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="5"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+    </row>
+    <row r="21" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5" t="s">
+      <c r="B22" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="12"/>
+      <c r="B23" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C23" s="13"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
+    </row>
+    <row r="24" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="10"/>
+      <c r="B24" s="11"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
+    </row>
+    <row r="25" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
-    </row>
-    <row r="5" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="B26" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C26" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
+      <c r="D26" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B27" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C27" s="8"/>
+      <c r="D27" s="8"/>
+      <c r="E27" s="8"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="9"/>
+      <c r="B28" s="9"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="9"/>
+    </row>
+    <row r="29" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A30" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A31" s="7"/>
+      <c r="B31" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C31" s="8"/>
+      <c r="D31" s="8"/>
+      <c r="E31" s="8"/>
+    </row>
+    <row r="33" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9" s="3" t="s">
+    <row r="34" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A34" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="D9" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
-    </row>
-    <row r="12" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="5"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-    </row>
-    <row r="16" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="5"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-    </row>
-    <row r="20" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="12"/>
-      <c r="B22" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C22" s="13"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
-    </row>
-    <row r="23" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="10"/>
-      <c r="B23" s="11"/>
-      <c r="C23" s="11"/>
-      <c r="D23" s="11"/>
-      <c r="E23" s="11"/>
-      <c r="F23" s="11"/>
-    </row>
-    <row r="24" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B25" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C26" s="8"/>
-      <c r="D26" s="8"/>
-      <c r="E26" s="8"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="9"/>
-      <c r="B27" s="9"/>
-      <c r="C27" s="9"/>
-      <c r="D27" s="9"/>
-      <c r="E27" s="9"/>
-      <c r="F27" s="9"/>
-    </row>
-    <row r="28" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="7"/>
-      <c r="B30" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C30" s="8"/>
-      <c r="D30" s="8"/>
-      <c r="E30" s="8"/>
-    </row>
-    <row r="32" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A33" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B33" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E33" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B34" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C34" s="5"/>
-      <c r="D34" s="5"/>
-      <c r="E34" s="5"/>
+      <c r="B35" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C35" s="5"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Hoàn thành 1 vài form thao tác
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TaiLieuHoc\LapTrinh(.)NET\DoAn_DotNet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AD0E592-B3E6-446A-A000-D37E072C5F2B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3606463A-CF2E-4928-8AC2-0B6C64D90CBA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{D266C75E-4EF3-451E-9F41-2CCBE411A25D}"/>
   </bookViews>
@@ -35,10 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="38">
-  <si>
-    <t>CMND</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="58">
   <si>
     <t>GIỚI TÍNH</t>
   </si>
@@ -52,16 +49,9 @@
     <t>TÊN</t>
   </si>
   <si>
-    <t>USER NAME</t>
-  </si>
-  <si>
     <t>PASSWORD</t>
   </si>
   <si>
-    <t>LOẠI 
-(ADMIN hoặc NV)</t>
-  </si>
-  <si>
     <t>LOẠI</t>
   </si>
   <si>
@@ -71,21 +61,12 @@
     <t>ĐỊA CHỈ</t>
   </si>
   <si>
-    <t>ĐƠN GIÁ</t>
-  </si>
-  <si>
     <t>KHÁCH HÀNG</t>
   </si>
   <si>
     <t>MÃ KH</t>
   </si>
   <si>
-    <t>MÃ AC</t>
-  </si>
-  <si>
-    <t>MÃ SP</t>
-  </si>
-  <si>
     <t>ĐƠN VỊ TÍNH</t>
   </si>
   <si>
@@ -101,9 +82,6 @@
     <t>NGÀY SINH</t>
   </si>
   <si>
-    <t>unique</t>
-  </si>
-  <si>
     <t>MÃ HD NHẬP</t>
   </si>
   <si>
@@ -125,9 +103,6 @@
     <t>MÃ LOẠI</t>
   </si>
   <si>
-    <t>Khóa ngoại</t>
-  </si>
-  <si>
     <t>TÊN LOẠI</t>
   </si>
   <si>
@@ -150,13 +125,171 @@
   </si>
   <si>
     <t>MÃ HH</t>
+  </si>
+  <si>
+    <t>NHANVIEN</t>
+  </si>
+  <si>
+    <t>Nvarchar(50) not null</t>
+  </si>
+  <si>
+    <t>CCCD</t>
+  </si>
+  <si>
+    <t>varchar(12) not null</t>
+  </si>
+  <si>
+    <t>bit not null</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>image</t>
+  </si>
+  <si>
+    <t>USERNAME</t>
+  </si>
+  <si>
+    <t>varchar(32) PK</t>
+  </si>
+  <si>
+    <t>varchar (12) not null</t>
+  </si>
+  <si>
+    <t>varchar(3) not null</t>
+  </si>
+  <si>
+    <t>varchar(5) PK</t>
+  </si>
+  <si>
+    <t>Nvarchar(30) not null</t>
+  </si>
+  <si>
+    <t>Ntext</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">varchar (5) </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>PK</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">varchar(5) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>FK</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">varchar(5) </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>PK</t>
+    </r>
+  </si>
+  <si>
+    <t>TÊN NCC</t>
+  </si>
+  <si>
+    <t>QUYỀN</t>
+  </si>
+  <si>
+    <t>MÃ NV</t>
+  </si>
+  <si>
+    <t>tinyint</t>
+  </si>
+  <si>
+    <t>smallmoney</t>
+  </si>
+  <si>
+    <t>Nvarchar(10)</t>
+  </si>
+  <si>
+    <t>datetime not null</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">varchar(9) </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>PK</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">varchar(9) </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>FK</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">varchar (5) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>FK</t>
+    </r>
+  </si>
+  <si>
+    <t>chưa cần</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -185,8 +318,22 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -211,8 +358,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -235,17 +388,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -260,9 +402,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -287,11 +426,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -607,20 +749,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D22EC28-166D-4546-9605-48C0E8032621}">
-  <dimension ref="A1:J35"/>
+  <dimension ref="A1:J49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.85546875" customWidth="1"/>
-    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.85546875" customWidth="1"/>
+    <col min="6" max="6" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="22.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.42578125" bestFit="1" customWidth="1"/>
@@ -629,7 +770,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -641,329 +782,501 @@
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
     </row>
-    <row r="2" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+    <row r="2" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="F2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+    </row>
+    <row r="3" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+    </row>
+    <row r="4" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="6"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+    </row>
+    <row r="5" spans="1:10" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+    </row>
+    <row r="6" spans="1:10" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+    </row>
+    <row r="7" spans="1:10" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C7" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+    </row>
+    <row r="8" spans="1:10" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+    </row>
+    <row r="10" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:10" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11"/>
+      <c r="C11"/>
+      <c r="D11"/>
+    </row>
+    <row r="12" spans="1:10" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+    </row>
+    <row r="16" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="4"/>
+      <c r="B19" s="4"/>
+    </row>
+    <row r="21" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I22" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="J22" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="B23" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="D23" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E23" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="F23" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="G23" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="H23" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="I23" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="J23" s="14" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="4"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="4"/>
+      <c r="H24" s="4"/>
+      <c r="I24" s="4"/>
+      <c r="J24" s="15" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C27" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D27" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" s="3" t="s">
+      <c r="E27" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A28" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="B28" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="C28" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="D28" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="E28" s="14" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" s="4"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+    </row>
+    <row r="31" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A32" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A33" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="B33" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="C33" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="D33" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="E33" s="14" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A34" s="11"/>
+      <c r="B34" s="4"/>
+      <c r="C34" s="12"/>
+      <c r="D34" s="12"/>
+      <c r="E34" s="12"/>
+    </row>
+    <row r="35" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A35" s="9"/>
+      <c r="B35" s="10"/>
+      <c r="C35" s="10"/>
+      <c r="D35" s="10"/>
+      <c r="E35" s="10"/>
+      <c r="F35" s="10"/>
+    </row>
+    <row r="36" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A37" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C37" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="7"/>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="14"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="5"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-    </row>
-    <row r="6" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D10" s="3" t="s">
+      <c r="D37" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A38" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="B38" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="C38" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="D38" s="14" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A39" s="4"/>
+      <c r="B39" s="4"/>
+      <c r="C39" s="7"/>
+      <c r="D39" s="7"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="8"/>
+      <c r="B40" s="8"/>
+      <c r="C40" s="8"/>
+      <c r="D40" s="8"/>
+      <c r="E40" s="8"/>
+      <c r="F40" s="8"/>
+    </row>
+    <row r="41" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A42" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C42" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E10" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="G10" s="3" t="s">
+      <c r="D42" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E42" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="H10" s="3" t="s">
+    </row>
+    <row r="43" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A43" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="B43" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="C43" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="D43" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="E43" s="14" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A44" s="6"/>
+      <c r="B44" s="7"/>
+      <c r="C44" s="7"/>
+      <c r="D44" s="7"/>
+      <c r="E44" s="7"/>
+    </row>
+    <row r="46" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A47" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I10" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="J10" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="5"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5" t="s">
+      <c r="B47" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="5"/>
-    </row>
-    <row r="13" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="5"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-    </row>
-    <row r="17" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
+      <c r="C47" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D47" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="5"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-    </row>
-    <row r="21" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="12"/>
-      <c r="B23" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C23" s="13"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-    </row>
-    <row r="24" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="10"/>
-      <c r="B24" s="11"/>
-      <c r="C24" s="11"/>
-      <c r="D24" s="11"/>
-      <c r="E24" s="11"/>
-      <c r="F24" s="11"/>
-    </row>
-    <row r="25" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B26" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C27" s="8"/>
-      <c r="D27" s="8"/>
-      <c r="E27" s="8"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="9"/>
-      <c r="B28" s="9"/>
-      <c r="C28" s="9"/>
-      <c r="D28" s="9"/>
-      <c r="E28" s="9"/>
-      <c r="F28" s="9"/>
-    </row>
-    <row r="29" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="7"/>
-      <c r="B31" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C31" s="8"/>
-      <c r="D31" s="8"/>
-      <c r="E31" s="8"/>
-    </row>
-    <row r="33" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A34" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B34" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E34" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B35" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C35" s="5"/>
-      <c r="D35" s="5"/>
-      <c r="E35" s="5"/>
+    </row>
+    <row r="48" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A48" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="B48" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="C48" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="D48" s="14" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="4"/>
+      <c r="B49" s="4"/>
+      <c r="C49" s="4"/>
+      <c r="D49" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>